<commit_message>
adding in updated data
</commit_message>
<xml_diff>
--- a/gamma_cross_sections/io/outputs/data/cross_section.xlsx
+++ b/gamma_cross_sections/io/outputs/data/cross_section.xlsx
@@ -462,9 +462,15 @@
       <c r="B2" t="n">
         <v>31</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>1.236943580958959e-29</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2.030566044183256e-31</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6.652458721354297e-29</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -490,9 +496,15 @@
       <c r="B4" t="n">
         <v>81</v>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>2.478386258082563e-30</v>
+      </c>
+      <c r="D4" t="n">
+        <v>8.387702135562965e-32</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6.652458721354297e-29</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -501,9 +513,15 @@
       <c r="B5" t="n">
         <v>356</v>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>1.170192421180405e-30</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.051214936270436e-31</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6.652458721354297e-29</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -512,9 +530,15 @@
       <c r="B6" t="n">
         <v>511</v>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>1.077782430867818e-30</v>
+      </c>
+      <c r="D6" t="n">
+        <v>6.967254681851096e-32</v>
+      </c>
+      <c r="E6" t="n">
+        <v>6.652458721354297e-29</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -540,9 +564,15 @@
       <c r="B8" t="n">
         <v>1275</v>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>7.786602954091923e-31</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.766717201428916e-31</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6.652458721354297e-29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>